<commit_message>
Changes to ADCS masses
</commit_message>
<xml_diff>
--- a/Budgets.xlsx
+++ b/Budgets.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\AERO3760-Space-Engineering-2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10780" windowHeight="7390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="14460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
   <si>
     <t>Budgeting</t>
   </si>
@@ -255,9 +255,6 @@
     <t>https://www.adafruit.com/products/1714</t>
   </si>
   <si>
-    <t>3 to 5V, tiny amps</t>
-  </si>
-  <si>
     <t>2.8g</t>
   </si>
   <si>
@@ -273,39 +270,15 @@
     <t>Good beginner user manual with setup arduino code</t>
   </si>
   <si>
-    <t>Pololu MinIMU-9 v3</t>
-  </si>
-  <si>
-    <t>//www.pololu.com/product/2468</t>
-  </si>
-  <si>
-    <t>Min operational 2.5V, max 5.5V, 6mA</t>
-  </si>
-  <si>
-    <t>0.7g</t>
-  </si>
-  <si>
-    <t>Uses pretty much same main technology as Adafruit</t>
-  </si>
-  <si>
-    <t>Almost certainly not as easy to interface with</t>
-  </si>
-  <si>
     <t>Photodiodes</t>
   </si>
   <si>
     <t>OSRAM SFH203P PHOTODIODE</t>
   </si>
   <si>
-    <t>$25 -$30</t>
-  </si>
-  <si>
     <t>-40 to 100</t>
   </si>
   <si>
-    <t>10-12g</t>
-  </si>
-  <si>
     <t>Will need either 5 or 6 which is reason for variation in price and weight.</t>
   </si>
   <si>
@@ -318,15 +291,6 @@
     <t>Air Core Magnetorquer</t>
   </si>
   <si>
-    <t>Copper Wire (Square or Round)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Between 3.3V and 5V </t>
-  </si>
-  <si>
-    <t>~60g</t>
-  </si>
-  <si>
     <t>Unsure of exact weight requirements will depend of mass of satellite</t>
   </si>
   <si>
@@ -397,17 +361,39 @@
   </si>
   <si>
     <t>RBF pin (buts power to satellite)</t>
+  </si>
+  <si>
+    <t>150mW</t>
+  </si>
+  <si>
+    <t>Copper Wire Round 0.18mm approx AWG 33</t>
+  </si>
+  <si>
+    <t>1.8g*6 (one on each face)</t>
+  </si>
+  <si>
+    <t>Approx 30mW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size 8cm by 8cm </t>
+  </si>
+  <si>
+    <t>Only if you can fit this</t>
+  </si>
+  <si>
+    <t>66g total (22g each)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -438,6 +424,12 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -462,10 +454,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -475,8 +469,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,7 +532,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,7 +567,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,7 +744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -757,22 +754,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" customWidth="1"/>
-    <col min="4" max="4" width="38.08984375" customWidth="1"/>
-    <col min="7" max="7" width="39.54296875" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -780,7 +780,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -788,7 +788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -796,7 +796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -804,7 +804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -824,10 +824,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -835,7 +835,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -855,7 +855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -869,7 +869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -886,7 +886,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -903,7 +903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -926,7 +926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -949,7 +949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -972,7 +972,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>42</v>
       </c>
@@ -986,7 +986,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>45</v>
@@ -995,18 +995,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="G21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="12">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="12">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -1060,12 +1060,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12">
       <c r="G28" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="12">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1096,15 +1096,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="12">
       <c r="A32" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="12">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12">
       <c r="B41" s="2" t="s">
         <v>70</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12">
       <c r="A42" s="2" t="s">
         <v>72</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>27.239429984372805</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12">
       <c r="A43" s="2" t="s">
         <v>73</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>54.47885996874561</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="12">
       <c r="A45" s="1" t="s">
         <v>74</v>
       </c>
@@ -1180,13 +1180,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="12">
       <c r="A46" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
@@ -1197,215 +1197,209 @@
         <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:7" ht="12">
+      <c r="G48" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="G48" s="2" t="s">
+    <row r="49" spans="1:7" ht="12">
+      <c r="G49" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="G49" s="2" t="s">
+    <row r="50" spans="1:7" ht="12">
+      <c r="G50" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="G50" s="2" t="s">
+    <row r="51" spans="1:7" ht="12">
+      <c r="A51" s="7"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" ht="12">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="54" spans="1:7" ht="12">
+      <c r="A54" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="B54" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C54" s="9">
+        <v>30</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="3">
-        <v>20</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="F54" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F51" s="2" t="s">
+    </row>
+    <row r="55" spans="1:7" ht="12">
+      <c r="G55" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="2" t="s">
+    </row>
+    <row r="57" spans="1:7" ht="12">
+      <c r="A57" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="G52" s="2" t="s">
+    <row r="58" spans="1:7" ht="12">
+      <c r="A58" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="B58" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="8" t="s">
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="12">
+      <c r="A60" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="61" spans="1:7" ht="12">
+      <c r="A61" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E54" s="2" t="s">
+    </row>
+    <row r="64" spans="1:7" ht="12">
+      <c r="A64" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="2" t="s">
+    </row>
+    <row r="65" spans="1:1" ht="12">
+      <c r="A65" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G54" s="2" t="s">
+    </row>
+    <row r="66" spans="1:1" ht="12">
+      <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="G55" s="2" t="s">
+    <row r="68" spans="1:1" ht="12">
+      <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="69" spans="1:1" ht="12">
+      <c r="A69" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="71" spans="1:1" ht="12">
+      <c r="A71" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="2" t="s">
+    </row>
+    <row r="72" spans="1:1" ht="12">
+      <c r="A72" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D58" s="2" t="s">
+    </row>
+    <row r="76" spans="1:1" ht="12">
+      <c r="A76" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F58" s="2" t="s">
+    </row>
+    <row r="78" spans="1:1" ht="12">
+      <c r="A78" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G58" s="2" t="s">
+    </row>
+    <row r="79" spans="1:1" ht="12">
+      <c r="A79" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="81" spans="1:1" ht="12">
+      <c r="A81" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="83" spans="1:1" ht="12">
+      <c r="A83" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="85" spans="1:1" ht="12">
+      <c r="A85" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="86" spans="1:1" ht="12">
+      <c r="A86" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="87" spans="1:1" ht="12">
+      <c r="A87" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="89" spans="1:1" ht="12">
+      <c r="A89" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="90" spans="1:1" ht="12">
+      <c r="A90" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="91" spans="1:1" ht="12">
+      <c r="A91" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+    <row r="93" spans="1:1" ht="12">
+      <c r="A93" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="94" spans="1:1" ht="12">
+      <c r="A94" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="95" spans="1:1" ht="12">
+      <c r="A95" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1425,5 +1419,11 @@
     <hyperlink ref="A72" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change to Power Requirements for Magnetorquers
</commit_message>
<xml_diff>
--- a/Budgets.xlsx
+++ b/Budgets.xlsx
@@ -363,9 +363,6 @@
     <t>RBF pin (buts power to satellite)</t>
   </si>
   <si>
-    <t>150mW</t>
-  </si>
-  <si>
     <t>Copper Wire Round 0.18mm approx AWG 33</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>66g total (22g each)</t>
+  </si>
+  <si>
+    <t>165mW</t>
   </si>
 </sst>
 </file>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1197,7 +1197,7 @@
         <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>78</v>
@@ -1246,7 +1246,7 @@
         <v>85</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>86</v>
@@ -1267,16 +1267,16 @@
         <v>89</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>90</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="E59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="12">

</xml_diff>